<commit_message>
working program with keys
</commit_message>
<xml_diff>
--- a/output/df_results.xlsx
+++ b/output/df_results.xlsx
@@ -8,48 +8,82 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446E8613-8A9E-4842-9F3E-A196FFA86073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696A9DC5-F62B-4EDB-8BCF-8C9782ADEF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>HOURS</t>
   </si>
   <si>
-    <t>E_demand</t>
-  </si>
-  <si>
-    <t>E_solar</t>
+    <t>P_demand</t>
+  </si>
+  <si>
+    <t>P_solar</t>
+  </si>
+  <si>
+    <t>P_buy</t>
+  </si>
+  <si>
+    <t>P_sell</t>
+  </si>
+  <si>
+    <t>P_bat_demand</t>
+  </si>
+  <si>
+    <t>P_bat_ch</t>
+  </si>
+  <si>
+    <t>P_bat_dis</t>
+  </si>
+  <si>
+    <t>P_bat_sell</t>
+  </si>
+  <si>
+    <t>P_pv_bat</t>
+  </si>
+  <si>
+    <t>P_pv_demand</t>
+  </si>
+  <si>
+    <t>P_pv_sell</t>
+  </si>
+  <si>
+    <t>E_sell</t>
   </si>
   <si>
     <t>E_buy</t>
   </si>
   <si>
-    <t>E_sell</t>
-  </si>
-  <si>
-    <t>E_bat</t>
-  </si>
-  <si>
-    <t>E_bat_demand</t>
-  </si>
-  <si>
-    <t>E_pv_bat</t>
-  </si>
-  <si>
-    <t>E_pv_demand</t>
-  </si>
-  <si>
-    <t>E_pv_sell</t>
+    <t>SOC</t>
+  </si>
+  <si>
+    <t>K_ch</t>
+  </si>
+  <si>
+    <t>K_dis</t>
   </si>
   <si>
     <t>1</t>
@@ -523,59 +557,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="9.26171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.26171875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.9453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.20703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.20703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.26171875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.05078125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>485</v>
@@ -584,30 +633,55 @@
         <v>893</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <f>C2*0.1</f>
+        <v>89.300000000000011</v>
       </c>
       <c r="E2">
-        <v>458.1</v>
+        <v>382.49999999999989</v>
       </c>
       <c r="F2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>485</v>
+        <v>13.200000000000021</v>
       </c>
       <c r="H2">
-        <v>435</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>13.200000000000021</v>
       </c>
       <c r="J2">
-        <v>458.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>89.300000000000011</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>382.49999999999989</v>
+      </c>
+      <c r="P2">
+        <v>0.5</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>444</v>
@@ -616,30 +690,55 @@
         <v>632</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <f t="shared" ref="D3:D25" si="0">C3*0.1</f>
+        <v>63.2</v>
       </c>
       <c r="E3">
-        <v>88.100000000000023</v>
+        <v>444</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>63.200000000000017</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>63.200000000000017</v>
+      </c>
+      <c r="L3">
+        <v>-1.4210854715202001E-14</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
         <v>444</v>
       </c>
-      <c r="H3">
-        <v>544</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>88.100000000000023</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="P3">
+        <v>0.36799999999999983</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>384</v>
@@ -648,30 +747,55 @@
         <v>212</v>
       </c>
       <c r="D4">
-        <v>71.899999999999977</v>
+        <f t="shared" si="0"/>
+        <v>21.200000000000003</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>262.8</v>
       </c>
       <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>100</v>
       </c>
-      <c r="G4">
-        <v>312.10000000000002</v>
-      </c>
       <c r="H4">
-        <v>212.1</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>21.2</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>262.8</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>325</v>
@@ -680,30 +804,55 @@
         <v>580</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>58</v>
       </c>
       <c r="E5">
-        <v>255.1</v>
+        <v>325</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>58.000000000000007</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>58.000000000000007</v>
+      </c>
+      <c r="L5">
+        <v>-1.4210854715202001E-14</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
         <v>325</v>
       </c>
-      <c r="H5">
-        <v>325</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>255.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>394</v>
@@ -712,30 +861,55 @@
         <v>607</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>60.7</v>
       </c>
       <c r="E6">
-        <v>113.1</v>
+        <v>275.3</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>394</v>
+        <v>58.000000000000021</v>
       </c>
       <c r="H6">
-        <v>494</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>58.000000000000021</v>
       </c>
       <c r="J6">
-        <v>113.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>60.7</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>275.3</v>
+      </c>
+      <c r="P6">
+        <v>0.58000000000000018</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>436</v>
@@ -744,19 +918,20 @@
         <v>177</v>
       </c>
       <c r="D7">
-        <v>158.9</v>
+        <f t="shared" si="0"/>
+        <v>17.7</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>436</v>
       </c>
       <c r="F7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>277.10000000000002</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>177.1</v>
+        <v>17.7</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -764,10 +939,34 @@
       <c r="J7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K7">
+        <v>17.7</v>
+      </c>
+      <c r="L7">
+        <v>-3.5527136788005009E-15</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>436</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>423</v>
@@ -776,30 +975,55 @@
         <v>735</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>73.5</v>
       </c>
       <c r="E8">
-        <v>212.1</v>
+        <v>343.9</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>423</v>
+        <v>5.6000000000000263</v>
       </c>
       <c r="H8">
-        <v>523</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>5.6000000000000263</v>
       </c>
       <c r="J8">
-        <v>212.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>73.5</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>343.9</v>
+      </c>
+      <c r="P8">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>459</v>
@@ -808,30 +1032,55 @@
         <v>879</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>87.9</v>
       </c>
       <c r="E9">
-        <v>520.1</v>
+        <v>459</v>
       </c>
       <c r="F9">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>87.90000000000002</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>87.90000000000002</v>
+      </c>
+      <c r="L9">
+        <v>-1.4210854715202001E-14</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
         <v>459</v>
       </c>
-      <c r="H9">
-        <v>359</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>520.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="P9">
+        <v>0.1209999999999998</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>406</v>
@@ -840,30 +1089,55 @@
         <v>731</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>73.100000000000009</v>
       </c>
       <c r="E10">
-        <v>225.1</v>
+        <v>232.9</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>406</v>
+        <v>100</v>
       </c>
       <c r="H10">
-        <v>506</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J10">
-        <v>225.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>73.100000000000009</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>232.9</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>300</v>
@@ -872,19 +1146,20 @@
         <v>281</v>
       </c>
       <c r="D11">
-        <v>18.899999999999981</v>
+        <f t="shared" si="0"/>
+        <v>28.1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="F11">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>281.10000000000002</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>281.10000000000002</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -892,10 +1167,34 @@
       <c r="J11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K11">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="L11">
+        <v>-7.1054273576010019E-15</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>300</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>435</v>
@@ -904,30 +1203,55 @@
         <v>232</v>
       </c>
       <c r="D12">
-        <v>414.9</v>
+        <f t="shared" si="0"/>
+        <v>23.200000000000003</v>
       </c>
       <c r="E12">
-        <v>232.1</v>
+        <v>435</v>
       </c>
       <c r="F12">
-        <v>100</v>
+        <v>-3.5527136788005009E-15</v>
       </c>
       <c r="G12">
-        <v>20.100000000000019</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>23.20000000000001</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
-        <v>232.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>23.20000000000001</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>-3.5527136788005009E-15</v>
+      </c>
+      <c r="N12">
+        <v>-3.5527136788005009E-15</v>
+      </c>
+      <c r="O12">
+        <v>435</v>
+      </c>
+      <c r="P12">
+        <v>0.28100000000000008</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>470</v>
@@ -936,30 +1260,55 @@
         <v>390</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>39</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>379.7</v>
       </c>
       <c r="F13">
-        <v>79.899999999999977</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>470</v>
+        <v>51.300000000000011</v>
       </c>
       <c r="H13">
-        <v>390.1</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>51.300000000000011</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>39</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>379.7</v>
+      </c>
+      <c r="P13">
+        <v>0.51300000000000012</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B14">
         <v>343</v>
@@ -968,30 +1317,55 @@
         <v>883</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>88.300000000000011</v>
       </c>
       <c r="E14">
-        <v>440.1</v>
+        <v>254.7</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>343</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>443</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14">
-        <v>440.1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>88.300000000000011</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>254.7</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B15">
         <v>485</v>
@@ -1000,30 +1374,55 @@
         <v>955</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>95.5</v>
       </c>
       <c r="E15">
-        <v>470.1</v>
+        <v>485</v>
       </c>
       <c r="F15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>95.500000000000014</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>95.500000000000014</v>
+      </c>
+      <c r="L15">
+        <v>-1.4210854715202001E-14</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
         <v>485</v>
       </c>
-      <c r="H15">
-        <v>485</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>470.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B16">
         <v>370</v>
@@ -1032,30 +1431,55 @@
         <v>841</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>84.100000000000009</v>
       </c>
       <c r="E16">
-        <v>571.1</v>
+        <v>290.39999999999998</v>
       </c>
       <c r="F16">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>370</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>270</v>
+        <v>4.4999999999999858</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>571.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>4.4999999999999858</v>
+      </c>
+      <c r="L16">
+        <v>79.600000000000023</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>290.39999999999998</v>
+      </c>
+      <c r="P16">
+        <v>0.95500000000000018</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <v>381</v>
@@ -1064,30 +1488,55 @@
         <v>385</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>38.5</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>275.3</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>381</v>
+        <v>67.200000000000017</v>
       </c>
       <c r="H17">
-        <v>385.1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>67.200000000000017</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>38.5</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>275.3</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B18">
         <v>397</v>
@@ -1096,30 +1545,55 @@
         <v>672</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>67.2</v>
       </c>
       <c r="E18">
-        <v>279.2</v>
+        <v>397</v>
       </c>
       <c r="F18">
-        <v>4.1000000000000227</v>
+        <v>0</v>
       </c>
       <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>67.200000000000017</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>67.200000000000017</v>
+      </c>
+      <c r="L18">
+        <v>-1.4210854715202001E-14</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
         <v>397</v>
       </c>
-      <c r="H18">
-        <v>392.9</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>279.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="P18">
+        <v>0.32799999999999979</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>363</v>
@@ -1128,30 +1602,55 @@
         <v>547</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>54.7</v>
       </c>
       <c r="E19">
-        <v>84.100000000000023</v>
+        <v>208.3</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>363</v>
+        <v>100</v>
       </c>
       <c r="H19">
-        <v>463</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J19">
-        <v>84.100000000000023</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>54.7</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>208.3</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B20">
         <v>436</v>
@@ -1160,30 +1659,55 @@
         <v>552</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>55.2</v>
       </c>
       <c r="E20">
-        <v>116.1</v>
+        <v>380.8</v>
       </c>
       <c r="F20">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>436</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>436</v>
+        <v>0</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20">
-        <v>116.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>55.2</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>380.8</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B21">
         <v>484</v>
@@ -1192,30 +1716,55 @@
         <v>976</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>97.600000000000009</v>
       </c>
       <c r="E21">
-        <v>592.1</v>
+        <v>484</v>
       </c>
       <c r="F21">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>97.600000000000037</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>97.600000000000037</v>
+      </c>
+      <c r="L21">
+        <v>-2.8421709430404007E-14</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
         <v>484</v>
       </c>
-      <c r="H21">
-        <v>384</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>592.1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>302</v>
@@ -1224,30 +1773,55 @@
         <v>734</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>73.400000000000006</v>
       </c>
       <c r="E22">
-        <v>370.2</v>
+        <v>230.99999999999989</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22">
-        <v>302</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>363.9</v>
+        <v>2.3999999999999631</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22">
-        <v>370.2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>2.3999999999999631</v>
+      </c>
+      <c r="L22">
+        <v>71.000000000000043</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>230.99999999999989</v>
+      </c>
+      <c r="P22">
+        <v>0.97600000000000042</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B23">
         <v>350</v>
@@ -1256,19 +1830,20 @@
         <v>388</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>38.800000000000004</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>311.2</v>
       </c>
       <c r="F23">
-        <v>61.899999999999977</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>388.1</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1276,10 +1851,34 @@
       <c r="J23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>311.2</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B24">
         <v>457</v>
@@ -1288,30 +1887,55 @@
         <v>731</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>73.100000000000009</v>
       </c>
       <c r="E24">
-        <v>374.1</v>
+        <v>283.89999999999998</v>
       </c>
       <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
         <v>100</v>
       </c>
-      <c r="G24">
-        <v>457</v>
-      </c>
       <c r="H24">
-        <v>357</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J24">
-        <v>374.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>73.100000000000009</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>283.89999999999998</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B25">
         <v>439</v>
@@ -1320,25 +1944,50 @@
         <v>754</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>75.400000000000006</v>
       </c>
       <c r="E25">
-        <v>754.1</v>
+        <v>263.60000000000002</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
-        <v>439</v>
+        <v>100</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J25">
-        <v>754.1</v>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>263.60000000000002</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>